<commit_message>
nmv 05 03 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS 1.8/Total stat for Kan 1 to 8.xlsx
+++ b/TS Jatai Ghanam Project/TS 1.8/Total stat for Kan 1 to 8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Ghanam Project\TS 1.8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\TS 1.8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Splits</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve"> PS+ Ruk</t>
   </si>
@@ -35,15 +32,6 @@
     <t>PG</t>
   </si>
   <si>
-    <t>Ruk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t>Ruks</t>
-  </si>
-  <si>
     <t>ELs</t>
   </si>
   <si>
@@ -90,6 +78,9 @@
   </si>
   <si>
     <t>Total Ghana / Jatai Vakyams</t>
+  </si>
+  <si>
+    <t>Total Ruks</t>
   </si>
 </sst>
 </file>
@@ -147,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -259,54 +250,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -359,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -378,10 +321,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,35 +339,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -719,7 +647,7 @@
     <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="1"/>
@@ -728,366 +656,340 @@
     <col min="12" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18" t="s">
+    <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2">
+        <v>234</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="2">
+        <v>58</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1530</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6">
+        <v>205</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>64</v>
+      </c>
+      <c r="H3" s="6">
         <v>3</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="I3" s="6">
+        <v>1690</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1914</v>
+      </c>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5">
+        <v>229</v>
+      </c>
+      <c r="D4" s="5">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>85</v>
+      </c>
+      <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2">
-        <v>234</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>58</v>
-      </c>
-      <c r="H3" s="2">
-        <v>6</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1530</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6">
-        <v>205</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6">
-        <v>24</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>64</v>
-      </c>
-      <c r="H4" s="6">
-        <v>3</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1690</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1914</v>
-      </c>
-      <c r="K4"/>
+      <c r="I4" s="5">
+        <v>1567</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1797</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="D5" s="5">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="5">
-        <v>85</v>
+        <v>163</v>
       </c>
       <c r="H5" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="5">
-        <v>1567</v>
+        <v>1810</v>
       </c>
       <c r="J5" s="5">
-        <v>1797</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5">
-        <v>285</v>
+        <v>369</v>
       </c>
       <c r="D6" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="H6" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I6" s="5">
-        <v>1810</v>
+        <v>2717</v>
       </c>
       <c r="J6" s="5">
-        <v>2085</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5">
         <v>51</v>
       </c>
       <c r="C7" s="5">
-        <v>369</v>
+        <v>416</v>
       </c>
       <c r="D7" s="5">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="H7" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I7" s="5">
-        <v>2717</v>
+        <v>2509</v>
       </c>
       <c r="J7" s="5">
-        <v>3087</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5">
+        <f>51</f>
         <v>51</v>
       </c>
       <c r="C8" s="5">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="D8" s="5">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="H8" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="5">
-        <v>2509</v>
+        <v>2655</v>
       </c>
       <c r="J8" s="5">
-        <v>2919</v>
+        <v>3073</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5">
-        <f>51</f>
-        <v>51</v>
-      </c>
-      <c r="C9" s="5">
-        <v>429</v>
-      </c>
-      <c r="D9" s="5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8">
+        <f>42</f>
+        <v>42</v>
+      </c>
+      <c r="C9" s="8">
+        <v>367</v>
+      </c>
+      <c r="D9" s="8">
         <v>22</v>
       </c>
-      <c r="E9" s="5">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>89</v>
-      </c>
-      <c r="H9" s="5">
+      <c r="E9" s="8">
+        <v>16</v>
+      </c>
+      <c r="F9" s="8">
         <v>5</v>
       </c>
-      <c r="I9" s="5">
-        <v>2655</v>
-      </c>
-      <c r="J9" s="5">
-        <v>3073</v>
+      <c r="G9" s="8">
+        <v>108</v>
+      </c>
+      <c r="H9" s="8">
+        <v>4</v>
+      </c>
+      <c r="I9" s="8">
+        <v>2094</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2450</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="8">
-        <f>42</f>
-        <v>42</v>
-      </c>
-      <c r="C10" s="8">
-        <v>367</v>
-      </c>
-      <c r="D10" s="8">
-        <v>22</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="8">
-        <v>5</v>
-      </c>
-      <c r="G10" s="8">
-        <v>108</v>
-      </c>
-      <c r="H10" s="8">
-        <v>4</v>
-      </c>
-      <c r="I10" s="8">
-        <v>2094</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="22">
-        <f>SUM(B3:B10)</f>
+      <c r="B10" s="16">
+        <f>SUM(B2:B9)</f>
         <v>342</v>
       </c>
-      <c r="C11" s="22">
-        <f t="shared" ref="C11:J11" si="0">SUM(C3:C10)</f>
+      <c r="C10" s="16">
+        <f t="shared" ref="C10:J10" si="0">SUM(C2:C9)</f>
         <v>2534</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D10" s="16">
         <f t="shared" si="0"/>
         <v>137</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E10" s="17">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>782</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H10" s="17">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I10" s="17">
         <f t="shared" si="0"/>
         <v>16572</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J10" s="17">
         <f t="shared" si="0"/>
         <v>19096</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>